<commit_message>
Checking in the new classes for Excel Reader
</commit_message>
<xml_diff>
--- a/src/test/resources/testFile.xlsx
+++ b/src/test/resources/testFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MyGround\excelPlay\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub-MyRepo\ExcelPlay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81331105-9C07-4408-B3F4-6DD1D3ADA094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FD4C4F-E42C-4C24-9136-3D536058054E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="2940" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>First Name</t>
   </si>
@@ -127,36 +127,6 @@
     <t>RollNo</t>
   </si>
   <si>
-    <t>Sno</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>32</t>
   </si>
   <si>
@@ -178,9 +148,6 @@
     <t>27</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>1562</t>
   </si>
   <si>
@@ -205,12 +172,6 @@
     <t>2456</t>
   </si>
   <si>
-    <t>6548</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>fnam1</t>
   </si>
   <si>
@@ -232,38 +193,76 @@
     <t>1454</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>fnam2</t>
-  </si>
-  <si>
-    <t>Lnam2</t>
-  </si>
-  <si>
-    <t>1457</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>fnam3</t>
-  </si>
-  <si>
-    <t>Lnam3</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>1459</t>
+    <t>testMethod01</t>
+  </si>
+  <si>
+    <t>testMethod03</t>
+  </si>
+  <si>
+    <t>testMethod04</t>
+  </si>
+  <si>
+    <t>testMethod05</t>
+  </si>
+  <si>
+    <t>testMethod06</t>
+  </si>
+  <si>
+    <t>testMethod07</t>
+  </si>
+  <si>
+    <t>testMethod08</t>
+  </si>
+  <si>
+    <t>testMethod02</t>
+  </si>
+  <si>
+    <t>testMethod09</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>TestMethodName</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -598,330 +597,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="16.6640625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="19.77734375" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.44140625" collapsed="false"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="3" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="G10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="H10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="I10" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>